<commit_message>
Added as.factor(Pop) and (Family)- keep that even if I revert from herbivory as glmer binomial... getting errors saying my models are too complex for my data, I think... Anyway changed 2019 herbivory models to glmer and got partway through 2020 July models before got so many error messages I'm taking a break so I can get help before continuing
</commit_message>
<xml_diff>
--- a/Figures_Tables/ranova_PVE/2019_2020_PVE_All.xlsx
+++ b/Figures_Tables/ranova_PVE/2019_2020_PVE_All.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbrei\Documents\R_Projects\chapter_two\Figures_Tables\ranova_PVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32426D6-7F90-4BE6-B54A-319FA88877CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A3EDDD3-7E61-4E0D-A9A7-EDBEAD6E79D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2020" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="42">
   <si>
     <t>Group</t>
   </si>
@@ -530,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -607,6 +607,10 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -637,12 +641,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -655,11 +653,12 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1216,7 +1215,7 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="N7" s="86" t="s">
+      <c r="N7" s="69" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2704,10 +2703,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E113D0C-DEAC-4D25-B90A-A8F8760B4604}">
-  <dimension ref="A2:M127"/>
+  <dimension ref="A2:M112"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2732,16 +2731,16 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C3" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="83" t="s">
+      <c r="C3" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="66" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2789,7 +2788,7 @@
       <c r="E6" s="11">
         <v>0.90595307199999997</v>
       </c>
-      <c r="M6" s="86" t="s">
+      <c r="M6" s="69" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2805,16 +2804,16 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C9" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="83" t="s">
+      <c r="C9" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="82" t="s">
+      <c r="F9" s="66" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2872,7 +2871,7 @@
       <c r="C14" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="82" t="s">
+      <c r="D14" s="66" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="12"/>
@@ -2900,16 +2899,16 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C18" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D18" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="83" t="s">
+      <c r="C18" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F18" s="82" t="s">
+      <c r="F18" s="66" t="s">
         <v>8</v>
       </c>
     </row>
@@ -2973,16 +2972,16 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C24" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" s="83" t="s">
+      <c r="C24" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="82" t="s">
+      <c r="F24" s="66" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3041,7 +3040,7 @@
       <c r="C29" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="82" t="s">
+      <c r="D29" s="66" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="12"/>
@@ -3069,16 +3068,16 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C34" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D34" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34" s="83" t="s">
+      <c r="C34" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F34" s="82" t="s">
+      <c r="F34" s="66" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3095,7 +3094,7 @@
       <c r="E35" s="12">
         <v>0.10939315729933</v>
       </c>
-      <c r="F35" s="85" t="s">
+      <c r="F35" s="68" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3139,16 +3138,16 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C40" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40" s="83" t="s">
+      <c r="C40" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="82" t="s">
+      <c r="F40" s="66" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3206,7 +3205,7 @@
       <c r="C45" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="82" t="s">
+      <c r="D45" s="66" t="s">
         <v>8</v>
       </c>
       <c r="E45" s="12"/>
@@ -3230,38 +3229,38 @@
         <v>13</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C50" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D50" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E50" s="83" t="s">
+      <c r="C50" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F50" s="82" t="s">
+      <c r="F50" s="66" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C51" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="1">
-        <v>0</v>
-      </c>
-      <c r="E51" s="11">
-        <v>0</v>
-      </c>
-      <c r="F51" s="1">
-        <v>1</v>
+      <c r="D51" s="4">
+        <v>2.0333907596472098E-5</v>
+      </c>
+      <c r="E51" s="12">
+        <v>7.9550613067627493E-2</v>
+      </c>
+      <c r="F51" s="4">
+        <v>7.9121335832738199E-3</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -3272,13 +3271,13 @@
         <v>3</v>
       </c>
       <c r="D52" s="1">
-        <v>0</v>
+        <v>1.9756837515539299E-6</v>
       </c>
       <c r="E52" s="11">
-        <v>0</v>
+        <v>7.7292990989657603E-3</v>
       </c>
       <c r="F52" s="1">
-        <v>1</v>
+        <v>0.64501010841093898</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -3286,10 +3285,10 @@
         <v>4</v>
       </c>
       <c r="D53" s="1">
-        <v>139.45854220499501</v>
+        <v>2.33300099292395E-4</v>
       </c>
       <c r="E53" s="11">
-        <v>1</v>
+        <v>0.91272008783340697</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -3300,38 +3299,38 @@
         <v>13</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C56" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D56" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E56" s="83" t="s">
+      <c r="C56" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F56" s="82" t="s">
+      <c r="F56" s="66" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="84" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D57" s="1">
-        <v>1.8544222161419801</v>
-      </c>
-      <c r="E57" s="11">
-        <v>1.6681916838342001E-2</v>
-      </c>
-      <c r="F57" s="1">
-        <v>0.74759777594751398</v>
+      <c r="D57" s="4">
+        <v>1.96126702482657E-5</v>
+      </c>
+      <c r="E57" s="12">
+        <v>7.7339227936591703E-2</v>
+      </c>
+      <c r="F57" s="4">
+        <v>3.2121049602536797E-2</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3342,13 +3341,13 @@
         <v>3</v>
       </c>
       <c r="D58" s="1">
-        <v>5.8355125577510497E-6</v>
+        <v>2.1845712254236701E-6</v>
       </c>
       <c r="E58" s="11">
-        <v>5.2494806387743598E-8</v>
+        <v>8.6144849124611504E-3</v>
       </c>
       <c r="F58" s="1">
-        <v>1</v>
+        <v>0.64717230983153695</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3356,10 +3355,10 @@
         <v>4</v>
       </c>
       <c r="D59" s="1">
-        <v>109.30918906216201</v>
+        <v>2.3179554412206999E-4</v>
       </c>
       <c r="E59" s="11">
-        <v>0.98331803066685197</v>
+        <v>0.91404628715094705</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
@@ -3371,677 +3370,514 @@
       <c r="C61" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="82" t="s">
+      <c r="D61" s="66" t="s">
         <v>8</v>
       </c>
       <c r="E61" s="12"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C62" s="1">
-        <v>2.0144072889008</v>
-      </c>
-      <c r="D62" s="1">
-        <v>0.155812106094359</v>
-      </c>
-      <c r="E62" s="12"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="B62" t="s">
+        <v>14</v>
+      </c>
+      <c r="C62" s="4">
+        <v>9.1162724615104604</v>
+      </c>
+      <c r="D62" s="4">
+        <v>2.5334566690482499E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>10</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B66" t="s">
         <v>13</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C65" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D65" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E65" s="83" t="s">
+      <c r="C66" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C67" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F65" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B66" t="s">
+      <c r="F67" s="66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
         <v>14</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C68" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D66" s="4">
-        <v>2.0333907596472098E-5</v>
-      </c>
-      <c r="E66" s="12">
-        <v>7.9550613067627493E-2</v>
-      </c>
-      <c r="F66" s="4">
-        <v>7.9121335832738199E-3</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B67" t="s">
+      <c r="D68" s="4">
+        <v>0.245723158179663</v>
+      </c>
+      <c r="E68" s="12">
+        <v>5.6088439068748497E-2</v>
+      </c>
+      <c r="F68" s="4">
+        <v>4.5453385163978198E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
         <v>16</v>
       </c>
-      <c r="C67" s="1" t="s">
+      <c r="C69" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D67" s="1">
-        <v>1.9756837515539299E-6</v>
-      </c>
-      <c r="E67" s="11">
-        <v>7.7292990989657603E-3</v>
-      </c>
-      <c r="F67" s="1">
-        <v>0.64501010841093898</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C68" s="1" t="s">
+      <c r="D69" s="1">
+        <v>9.7883362437808805E-2</v>
+      </c>
+      <c r="E69" s="11">
+        <v>2.2342725246609001E-2</v>
+      </c>
+      <c r="F69" s="1">
+        <v>0.17667658839320299</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C70" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D68" s="1">
-        <v>2.33300099292395E-4</v>
-      </c>
-      <c r="E68" s="11">
-        <v>0.91272008783340697</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+      <c r="D70" s="1">
+        <v>4.0373882487052501</v>
+      </c>
+      <c r="E70" s="11">
+        <v>0.92156883568464298</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>11</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B72" t="s">
         <v>13</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C71" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D71" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E71" s="83" t="s">
+      <c r="C72" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C73" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F71" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B72" t="s">
+      <c r="F73" s="66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
         <v>14</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C74" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D72" s="4">
-        <v>1.96126702482657E-5</v>
-      </c>
-      <c r="E72" s="12">
-        <v>7.7339227936591703E-2</v>
-      </c>
-      <c r="F72" s="4">
-        <v>3.2121049602536797E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B73" t="s">
-        <v>16</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D73" s="1">
-        <v>2.1845712254236701E-6</v>
-      </c>
-      <c r="E73" s="11">
-        <v>8.6144849124611504E-3</v>
-      </c>
-      <c r="F73" s="1">
-        <v>0.64717230983153695</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C74" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D74" s="1">
-        <v>2.3179554412206999E-4</v>
-      </c>
-      <c r="E74" s="11">
-        <v>0.91404628715094705</v>
+      <c r="D74" s="4">
+        <v>0.33800426302070102</v>
+      </c>
+      <c r="E74" s="12">
+        <v>7.2009099967587795E-2</v>
+      </c>
+      <c r="F74" s="4">
+        <v>3.6760923246975503E-2</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C76" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D76" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E76" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="1">
+        <v>7.5453122078170301E-2</v>
+      </c>
+      <c r="E75" s="11">
+        <v>1.6074683088422501E-2</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0.42674233087998298</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C76" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="1">
+        <v>4.2804530119598496</v>
+      </c>
+      <c r="E76" s="11">
+        <v>0.91191621694399005</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C78" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D78" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="12"/>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
         <v>14</v>
       </c>
-      <c r="C77" s="4">
-        <v>9.1162724615104604</v>
-      </c>
-      <c r="D77" s="4">
-        <v>2.5334566690482499E-3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+      <c r="C79" s="4">
+        <v>5.8869673558654796</v>
+      </c>
+      <c r="D79" s="4">
+        <v>1.52533462997322E-2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
         <v>10</v>
       </c>
-      <c r="B81" t="s">
+      <c r="B83" t="s">
         <v>13</v>
       </c>
-      <c r="C81" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C82" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D82" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E82" s="83" t="s">
+      <c r="C83" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C84" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F82" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B83" t="s">
+      <c r="F84" s="66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
         <v>14</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C85" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D83" s="4">
-        <v>0.245723158179663</v>
-      </c>
-      <c r="E83" s="12">
-        <v>5.6088439068748497E-2</v>
-      </c>
-      <c r="F83" s="4">
-        <v>4.5453385163978198E-2</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B84" t="s">
+      <c r="D85" s="4">
+        <v>0.14885883450706699</v>
+      </c>
+      <c r="E85" s="12">
+        <v>7.6278263813371203E-2</v>
+      </c>
+      <c r="F85" s="4">
+        <v>1.2733827373075501E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
         <v>16</v>
       </c>
-      <c r="C84" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D84" s="1">
-        <v>9.7883362437808805E-2</v>
-      </c>
-      <c r="E84" s="11">
-        <v>2.2342725246609001E-2</v>
-      </c>
-      <c r="F84" s="1">
-        <v>0.17667658839320299</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C85" s="1" t="s">
+      <c r="D86" s="1">
+        <v>1.9659644007783202E-2</v>
+      </c>
+      <c r="E86" s="11">
+        <v>1.00739974020921E-2</v>
+      </c>
+      <c r="F86" s="1">
+        <v>0.57060192602450299</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C87" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D85" s="1">
-        <v>4.0373882487052501</v>
-      </c>
-      <c r="E85" s="11">
-        <v>0.92156883568464298</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
+      <c r="D87" s="1">
+        <v>1.7830051543680101</v>
+      </c>
+      <c r="E87" s="11">
+        <v>0.91364773878453698</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>11</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B89" t="s">
         <v>13</v>
       </c>
-      <c r="C87" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C88" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D88" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E88" s="83" t="s">
+      <c r="C89" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C90" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F88" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B89" t="s">
+      <c r="F90" s="66" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
         <v>14</v>
       </c>
-      <c r="C89" s="4" t="s">
+      <c r="C91" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D89" s="4">
-        <v>0.33800426302070102</v>
-      </c>
-      <c r="E89" s="12">
-        <v>7.2009099967587795E-2</v>
-      </c>
-      <c r="F89" s="4">
-        <v>3.6760923246975503E-2</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B90" t="s">
-        <v>16</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D90" s="1">
-        <v>7.5453122078170301E-2</v>
-      </c>
-      <c r="E90" s="11">
-        <v>1.6074683088422501E-2</v>
-      </c>
-      <c r="F90" s="1">
-        <v>0.42674233087998298</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C91" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D91" s="1">
-        <v>4.2804530119598496</v>
-      </c>
-      <c r="E91" s="11">
-        <v>0.91191621694399005</v>
+      <c r="D91" s="4">
+        <v>0.17864087030591899</v>
+      </c>
+      <c r="E91" s="12">
+        <v>7.9128109656400797E-2</v>
+      </c>
+      <c r="F91" s="4">
+        <v>3.51154997196974E-2</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C93" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D93" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E93" s="12"/>
+        <v>16</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" s="1">
+        <v>1.3029234944463499E-2</v>
+      </c>
+      <c r="E92" s="11">
+        <v>5.7712366137658497E-3</v>
+      </c>
+      <c r="F92" s="1">
+        <v>0.78586994844497404</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C93" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" s="1">
+        <v>2.0659456912299601</v>
+      </c>
+      <c r="E93" s="11">
+        <v>0.91510065372983296</v>
+      </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
-        <v>14</v>
-      </c>
-      <c r="C94" s="4">
-        <v>5.8869673558654796</v>
-      </c>
-      <c r="D94" s="4">
-        <v>1.52533462997322E-2</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C95" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D95" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E95" s="12"/>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>18</v>
+      </c>
+      <c r="C96" s="9">
+        <v>2.95703412277008</v>
+      </c>
+      <c r="D96" s="9">
+        <v>8.5504649253308904E-2</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
         <v>10</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B99" t="s">
         <v>13</v>
       </c>
-      <c r="C98" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C99" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D99" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E99" s="83" t="s">
+      <c r="C99" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C100" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E100" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F99" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B100" t="s">
-        <v>14</v>
-      </c>
-      <c r="C100" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" s="4">
-        <v>0.14885883450706699</v>
-      </c>
-      <c r="E100" s="12">
-        <v>7.6278263813371203E-2</v>
-      </c>
-      <c r="F100" s="4">
-        <v>1.2733827373075501E-2</v>
+      <c r="F100" s="66" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
+        <v>14</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D101" s="4">
+        <v>0.13915490094109101</v>
+      </c>
+      <c r="E101" s="12">
+        <v>8.3376391082875201E-2</v>
+      </c>
+      <c r="F101" s="4">
+        <v>2.5852583564641299E-3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
         <v>16</v>
       </c>
-      <c r="C101" s="1" t="s">
+      <c r="C102" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D101" s="1">
-        <v>1.9659644007783202E-2</v>
-      </c>
-      <c r="E101" s="11">
-        <v>1.00739974020921E-2</v>
-      </c>
-      <c r="F101" s="1">
-        <v>0.57060192602450299</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C102" s="1" t="s">
+      <c r="D102" s="1">
+        <v>0</v>
+      </c>
+      <c r="E102" s="11">
+        <v>0</v>
+      </c>
+      <c r="F102" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C103" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D102" s="1">
-        <v>1.7830051543680101</v>
-      </c>
-      <c r="E102" s="11">
-        <v>0.91364773878453698</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+      <c r="D103" s="1">
+        <v>1.52984155157714</v>
+      </c>
+      <c r="E103" s="11">
+        <v>0.91662360891712502</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
         <v>11</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B105" t="s">
         <v>13</v>
       </c>
-      <c r="C104" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C105" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D105" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E105" s="83" t="s">
+      <c r="C105" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C106" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E106" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="F105" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B106" t="s">
-        <v>14</v>
-      </c>
-      <c r="C106" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D106" s="4">
-        <v>0.17864087030591899</v>
-      </c>
-      <c r="E106" s="12">
-        <v>7.9128109656400797E-2</v>
-      </c>
-      <c r="F106" s="4">
-        <v>3.51154997196974E-2</v>
+      <c r="F106" s="66" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
+        <v>14</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D107" s="4">
+        <v>0.152029635203904</v>
+      </c>
+      <c r="E107" s="12">
+        <v>9.3418114805219804E-2</v>
+      </c>
+      <c r="F107" s="4">
+        <v>5.9721380767463004E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
         <v>16</v>
       </c>
-      <c r="C107" s="1" t="s">
+      <c r="C108" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D107" s="1">
-        <v>1.3029234944463499E-2</v>
-      </c>
-      <c r="E107" s="11">
-        <v>5.7712366137658497E-3</v>
-      </c>
-      <c r="F107" s="1">
-        <v>0.78586994844497404</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C108" s="1" t="s">
+      <c r="D108" s="1">
+        <v>1.9797624200162401E-8</v>
+      </c>
+      <c r="E108" s="11">
+        <v>1.21651066775294E-8</v>
+      </c>
+      <c r="F108" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C109" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D108" s="1">
-        <v>2.0659456912299601</v>
-      </c>
-      <c r="E108" s="11">
-        <v>0.91510065372983296</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B109" t="s">
+      <c r="D109" s="1">
+        <v>1.47538099785623</v>
+      </c>
+      <c r="E109" s="11">
+        <v>0.90658187302967397</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C110" s="4" t="s">
+    <row r="111" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C111" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D110" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E110" s="12"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B111" t="s">
-        <v>18</v>
-      </c>
-      <c r="C111" s="9">
-        <v>2.95703412277008</v>
-      </c>
-      <c r="D111" s="9">
-        <v>8.5504649253308904E-2</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>10</v>
-      </c>
-      <c r="B114" t="s">
-        <v>13</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C115" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D115" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E115" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="F115" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B116" t="s">
-        <v>14</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D116" s="4">
-        <v>0.13915490094109101</v>
-      </c>
-      <c r="E116" s="12">
-        <v>8.3376391082875201E-2</v>
-      </c>
-      <c r="F116" s="4">
-        <v>2.5852583564641299E-3</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B117" t="s">
+      <c r="D111" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E111" s="12"/>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
         <v>16</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D117" s="1">
-        <v>0</v>
-      </c>
-      <c r="E117" s="11">
-        <v>0</v>
-      </c>
-      <c r="F117" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C118" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D118" s="1">
-        <v>1.52984155157714</v>
-      </c>
-      <c r="E118" s="11">
-        <v>0.91662360891712502</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A120" t="s">
-        <v>11</v>
-      </c>
-      <c r="B120" t="s">
-        <v>13</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C121" s="82" t="s">
-        <v>0</v>
-      </c>
-      <c r="D121" s="82" t="s">
-        <v>1</v>
-      </c>
-      <c r="E121" s="83" t="s">
-        <v>2</v>
-      </c>
-      <c r="F121" s="82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B122" t="s">
-        <v>14</v>
-      </c>
-      <c r="C122" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D122" s="4">
-        <v>0.152029635203904</v>
-      </c>
-      <c r="E122" s="12">
-        <v>9.3418114805219804E-2</v>
-      </c>
-      <c r="F122" s="4">
-        <v>5.9721380767463004E-3</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B123" t="s">
-        <v>16</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D123" s="1">
-        <v>1.9797624200162401E-8</v>
-      </c>
-      <c r="E123" s="11">
-        <v>1.21651066775294E-8</v>
-      </c>
-      <c r="F123" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C124" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D124" s="1">
-        <v>1.47538099785623</v>
-      </c>
-      <c r="E124" s="11">
-        <v>0.90658187302967397</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B125" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C126" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D126" s="82" t="s">
-        <v>8</v>
-      </c>
-      <c r="E126" s="12"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B127" t="s">
-        <v>16</v>
-      </c>
-      <c r="C127" s="1">
+      <c r="C112" s="1">
         <v>6.9809500004895997E-2</v>
       </c>
-      <c r="D127" s="1">
+      <c r="D112" s="1">
         <v>0.79161434987560597</v>
       </c>
     </row>
@@ -4055,7 +3891,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77878847-70DC-4035-AFE6-61B1D9B32069}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B24" sqref="B24:B26"/>
     </sheetView>
   </sheetViews>
@@ -4079,30 +3915,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="15" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="75"/>
-      <c r="H1" s="73" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="79"/>
+      <c r="H1" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="66" t="s">
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="67"/>
+      <c r="N1" s="71"/>
       <c r="O1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="64" t="s">
         <v>6</v>
       </c>
@@ -4112,8 +3948,8 @@
       <c r="F2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="80"/>
-      <c r="I2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="83"/>
       <c r="J2" s="62" t="s">
         <v>6</v>
       </c>
@@ -4123,16 +3959,16 @@
       <c r="L2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="77"/>
+      <c r="N2" s="85"/>
       <c r="O2" s="37"/>
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="74" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="57" t="s">
@@ -4141,7 +3977,7 @@
       <c r="D3" s="48"/>
       <c r="E3" s="18"/>
       <c r="F3" s="19"/>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="74" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="57" t="s">
@@ -4160,14 +3996,14 @@
     </row>
     <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="71"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D4" s="48"/>
       <c r="E4" s="18"/>
       <c r="F4" s="19"/>
-      <c r="H4" s="71"/>
+      <c r="H4" s="75"/>
       <c r="I4" s="58" t="s">
         <v>26</v>
       </c>
@@ -4184,14 +4020,14 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="71"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="49"/>
       <c r="E5" s="20"/>
       <c r="F5" s="21"/>
-      <c r="H5" s="72"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="59" t="s">
         <v>8</v>
       </c>
@@ -4203,7 +4039,7 @@
       <c r="O5" s="39"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="74" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="57" t="s">
@@ -4212,7 +4048,7 @@
       <c r="D6" s="50"/>
       <c r="E6" s="16"/>
       <c r="F6" s="17"/>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="74" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="57" t="s">
@@ -4230,14 +4066,14 @@
       <c r="O6" s="39"/>
     </row>
     <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="51"/>
       <c r="E7" s="22"/>
       <c r="F7" s="23"/>
-      <c r="H7" s="71"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="58" t="s">
         <v>26</v>
       </c>
@@ -4254,14 +4090,14 @@
     </row>
     <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="72"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="52"/>
       <c r="E8" s="24"/>
       <c r="F8" s="25"/>
-      <c r="H8" s="72"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="59" t="s">
         <v>8</v>
       </c>
@@ -4274,7 +4110,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="57" t="s">
@@ -4283,7 +4119,7 @@
       <c r="D9" s="43"/>
       <c r="E9" s="27"/>
       <c r="F9" s="17"/>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="74" t="s">
         <v>20</v>
       </c>
       <c r="I9" s="57" t="s">
@@ -4301,14 +4137,14 @@
       <c r="O9" s="39"/>
     </row>
     <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="71"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D10" s="41"/>
       <c r="E10" s="22"/>
       <c r="F10" s="23"/>
-      <c r="H10" s="71"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="58" t="s">
         <v>26</v>
       </c>
@@ -4324,14 +4160,14 @@
       <c r="O10" s="39"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="72"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="53"/>
       <c r="E11" s="28"/>
       <c r="F11" s="25"/>
-      <c r="H11" s="72"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="59" t="s">
         <v>8</v>
       </c>
@@ -4344,7 +4180,7 @@
     </row>
     <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="57" t="s">
@@ -4353,7 +4189,7 @@
       <c r="D12" s="38"/>
       <c r="E12" s="16"/>
       <c r="F12" s="17"/>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="74" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="57" t="s">
@@ -4371,14 +4207,14 @@
       <c r="O12" s="39"/>
     </row>
     <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="71"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="41"/>
       <c r="E13" s="22"/>
       <c r="F13" s="23"/>
-      <c r="H13" s="71"/>
+      <c r="H13" s="75"/>
       <c r="I13" s="58" t="s">
         <v>26</v>
       </c>
@@ -4395,14 +4231,14 @@
     </row>
     <row r="14" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="72"/>
+      <c r="B14" s="76"/>
       <c r="C14" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="53"/>
       <c r="E14" s="24"/>
       <c r="F14" s="25"/>
-      <c r="H14" s="72"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="59" t="s">
         <v>8</v>
       </c>
@@ -4415,7 +4251,7 @@
     </row>
     <row r="15" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="74" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="57" t="s">
@@ -4424,7 +4260,7 @@
       <c r="D15" s="54"/>
       <c r="E15" s="30"/>
       <c r="F15" s="17"/>
-      <c r="H15" s="70" t="s">
+      <c r="H15" s="74" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="57" t="s">
@@ -4443,14 +4279,14 @@
     </row>
     <row r="16" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
-      <c r="B16" s="71"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="41"/>
       <c r="E16" s="22"/>
       <c r="F16" s="23"/>
-      <c r="H16" s="71"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="58" t="s">
         <v>26</v>
       </c>
@@ -4466,14 +4302,14 @@
       <c r="O16" s="39"/>
     </row>
     <row r="17" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="72"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="55"/>
       <c r="E17" s="28"/>
       <c r="F17" s="25"/>
-      <c r="H17" s="72"/>
+      <c r="H17" s="76"/>
       <c r="I17" s="59" t="s">
         <v>8</v>
       </c>
@@ -4486,7 +4322,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="74" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="57" t="s">
@@ -4495,7 +4331,7 @@
       <c r="D18" s="56"/>
       <c r="E18" s="33"/>
       <c r="F18" s="17"/>
-      <c r="H18" s="70" t="s">
+      <c r="H18" s="74" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="57" t="s">
@@ -4513,14 +4349,14 @@
       <c r="O18" s="39"/>
     </row>
     <row r="19" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="71"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="41"/>
       <c r="E19" s="22"/>
       <c r="F19" s="23"/>
-      <c r="H19" s="71"/>
+      <c r="H19" s="75"/>
       <c r="I19" s="58" t="s">
         <v>26</v>
       </c>
@@ -4536,14 +4372,14 @@
       <c r="O19" s="39"/>
     </row>
     <row r="20" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="72"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="42"/>
       <c r="E20" s="35"/>
       <c r="F20" s="25"/>
-      <c r="H20" s="72"/>
+      <c r="H20" s="76"/>
       <c r="I20" s="59" t="s">
         <v>8</v>
       </c>
@@ -4556,7 +4392,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="74" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="57" t="s">
@@ -4565,7 +4401,7 @@
       <c r="D21" s="56"/>
       <c r="E21" s="33"/>
       <c r="F21" s="26"/>
-      <c r="H21" s="70" t="s">
+      <c r="H21" s="74" t="s">
         <v>27</v>
       </c>
       <c r="I21" s="57" t="s">
@@ -4584,14 +4420,14 @@
     </row>
     <row r="22" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="71"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D22" s="41"/>
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
-      <c r="H22" s="71"/>
+      <c r="H22" s="75"/>
       <c r="I22" s="58" t="s">
         <v>26</v>
       </c>
@@ -4607,14 +4443,14 @@
       <c r="O22" s="39"/>
     </row>
     <row r="23" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="72"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="42"/>
       <c r="E23" s="35"/>
       <c r="F23" s="25"/>
-      <c r="H23" s="72"/>
+      <c r="H23" s="76"/>
       <c r="I23" s="59" t="s">
         <v>8</v>
       </c>
@@ -4627,7 +4463,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="74" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="57" t="s">
@@ -4636,7 +4472,7 @@
       <c r="D24" s="50"/>
       <c r="E24" s="16"/>
       <c r="F24" s="17"/>
-      <c r="H24" s="70" t="s">
+      <c r="H24" s="74" t="s">
         <v>29</v>
       </c>
       <c r="I24" s="57" t="s">
@@ -4655,14 +4491,14 @@
     </row>
     <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
-      <c r="B25" s="71"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D25" s="51"/>
       <c r="E25" s="22"/>
       <c r="F25" s="23"/>
-      <c r="H25" s="71"/>
+      <c r="H25" s="75"/>
       <c r="I25" s="58" t="s">
         <v>26</v>
       </c>
@@ -4678,14 +4514,14 @@
       <c r="O25" s="39"/>
     </row>
     <row r="26" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="72"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="52"/>
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
-      <c r="H26" s="72"/>
+      <c r="H26" s="76"/>
       <c r="I26" s="59" t="s">
         <v>8</v>
       </c>
@@ -4697,7 +4533,7 @@
       <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="74" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="57" t="s">
@@ -4706,7 +4542,7 @@
       <c r="D27" s="54"/>
       <c r="E27" s="16"/>
       <c r="F27" s="17"/>
-      <c r="H27" s="70" t="s">
+      <c r="H27" s="74" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="57" t="s">
@@ -4723,14 +4559,14 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="71"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="58" t="s">
         <v>26</v>
       </c>
       <c r="D28" s="41"/>
       <c r="E28" s="22"/>
       <c r="F28" s="23"/>
-      <c r="H28" s="71"/>
+      <c r="H28" s="75"/>
       <c r="I28" s="58" t="s">
         <v>26</v>
       </c>
@@ -4745,14 +4581,14 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="72"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="59" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="55"/>
       <c r="E29" s="24"/>
       <c r="F29" s="25"/>
-      <c r="H29" s="72"/>
+      <c r="H29" s="76"/>
       <c r="I29" s="59" t="s">
         <v>8</v>
       </c>
@@ -4805,19 +4641,37 @@
       <c r="C39" s="1"/>
     </row>
     <row r="70" spans="17:18" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q70" s="66" t="s">
+      <c r="Q70" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="R70" s="67"/>
+      <c r="R70" s="71"/>
     </row>
     <row r="71" spans="17:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q71" s="68" t="s">
+      <c r="Q71" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="R71" s="69"/>
+      <c r="R71" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="H9:H11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="H18:H20"/>
     <mergeCell ref="Q70:R70"/>
     <mergeCell ref="Q71:R71"/>
     <mergeCell ref="B21:B23"/>
@@ -4826,24 +4680,6 @@
     <mergeCell ref="H24:H26"/>
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="H27:H29"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="H18:H20"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="H9:H11"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="M2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4878,30 +4714,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="15" customFormat="1" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="74"/>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="75"/>
-      <c r="H1" s="73" t="s">
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="79"/>
+      <c r="H1" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="75"/>
-      <c r="M1" s="66" t="s">
+      <c r="I1" s="78"/>
+      <c r="J1" s="78"/>
+      <c r="K1" s="78"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="N1" s="67"/>
+      <c r="N1" s="71"/>
       <c r="O1" s="36"/>
     </row>
     <row r="2" spans="1:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6"/>
-      <c r="B2" s="78"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="81"/>
       <c r="D2" s="64" t="s">
         <v>6</v>
       </c>
@@ -4911,8 +4747,8 @@
       <c r="F2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="80"/>
-      <c r="I2" s="81"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="83"/>
       <c r="J2" s="62" t="s">
         <v>6</v>
       </c>
@@ -4922,16 +4758,16 @@
       <c r="L2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="76" t="s">
+      <c r="M2" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="77"/>
+      <c r="N2" s="85"/>
       <c r="O2" s="37"/>
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="74" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="57" t="s">
@@ -4946,7 +4782,7 @@
       <c r="F3" s="19">
         <v>921.24755427567402</v>
       </c>
-      <c r="H3" s="70" t="s">
+      <c r="H3" s="74" t="s">
         <v>7</v>
       </c>
       <c r="I3" s="57" t="s">
@@ -4971,7 +4807,7 @@
     </row>
     <row r="4" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="71"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="58" t="s">
         <v>26</v>
       </c>
@@ -4984,7 +4820,7 @@
       <c r="F4" s="19">
         <v>0.88365008222176999</v>
       </c>
-      <c r="H4" s="71"/>
+      <c r="H4" s="75"/>
       <c r="I4" s="58" t="s">
         <v>26</v>
       </c>
@@ -5007,7 +4843,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="71"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="59" t="s">
         <v>8</v>
       </c>
@@ -5018,7 +4854,7 @@
         <v>0.79796923089905303</v>
       </c>
       <c r="F5" s="21"/>
-      <c r="H5" s="72"/>
+      <c r="H5" s="76"/>
       <c r="I5" s="59" t="s">
         <v>8</v>
       </c>
@@ -5034,7 +4870,7 @@
       <c r="O5" s="39"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="70" t="s">
+      <c r="B6" s="74" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="57" t="s">
@@ -5049,7 +4885,7 @@
       <c r="F6" s="17">
         <v>4355.7927582254097</v>
       </c>
-      <c r="H6" s="70" t="s">
+      <c r="H6" s="74" t="s">
         <v>9</v>
       </c>
       <c r="I6" s="57" t="s">
@@ -5073,7 +4909,7 @@
       <c r="O6" s="39"/>
     </row>
     <row r="7" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="71"/>
+      <c r="B7" s="75"/>
       <c r="C7" s="58" t="s">
         <v>26</v>
       </c>
@@ -5086,7 +4922,7 @@
       <c r="F7" s="23">
         <v>0.93810572603869102</v>
       </c>
-      <c r="H7" s="71"/>
+      <c r="H7" s="75"/>
       <c r="I7" s="58" t="s">
         <v>26</v>
       </c>
@@ -5109,7 +4945,7 @@
     </row>
     <row r="8" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="72"/>
+      <c r="B8" s="76"/>
       <c r="C8" s="59" t="s">
         <v>8</v>
       </c>
@@ -5120,7 +4956,7 @@
         <v>0.57740693299851797</v>
       </c>
       <c r="F8" s="25"/>
-      <c r="H8" s="72"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="59" t="s">
         <v>8</v>
       </c>
@@ -5137,7 +4973,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="74" t="s">
         <v>20</v>
       </c>
       <c r="C9" s="57" t="s">
@@ -5152,7 +4988,7 @@
       <c r="F9" s="17">
         <v>1.52697992387702E-2</v>
       </c>
-      <c r="H9" s="70" t="s">
+      <c r="H9" s="74" t="s">
         <v>20</v>
       </c>
       <c r="I9" s="57" t="s">
@@ -5176,7 +5012,7 @@
       <c r="O9" s="39"/>
     </row>
     <row r="10" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="71"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="58" t="s">
         <v>26</v>
       </c>
@@ -5189,7 +5025,7 @@
       <c r="F10" s="23">
         <v>0.98768146963247405</v>
       </c>
-      <c r="H10" s="71"/>
+      <c r="H10" s="75"/>
       <c r="I10" s="58" t="s">
         <v>26</v>
       </c>
@@ -5211,7 +5047,7 @@
       <c r="O10" s="39"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="72"/>
+      <c r="B11" s="76"/>
       <c r="C11" s="59" t="s">
         <v>8</v>
       </c>
@@ -5222,7 +5058,7 @@
         <v>0.999982379273889</v>
       </c>
       <c r="F11" s="25"/>
-      <c r="H11" s="72"/>
+      <c r="H11" s="76"/>
       <c r="I11" s="59" t="s">
         <v>8</v>
       </c>
@@ -5239,7 +5075,7 @@
     </row>
     <row r="12" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="70" t="s">
+      <c r="B12" s="74" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="57" t="s">
@@ -5254,7 +5090,7 @@
       <c r="F12" s="17">
         <v>42.872105325543203</v>
       </c>
-      <c r="H12" s="70" t="s">
+      <c r="H12" s="74" t="s">
         <v>21</v>
       </c>
       <c r="I12" s="57" t="s">
@@ -5278,7 +5114,7 @@
       <c r="O12" s="39"/>
     </row>
     <row r="13" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="71"/>
+      <c r="B13" s="75"/>
       <c r="C13" s="58" t="s">
         <v>26</v>
       </c>
@@ -5291,7 +5127,7 @@
       <c r="F13" s="23">
         <v>0.98375453001832602</v>
       </c>
-      <c r="H13" s="71"/>
+      <c r="H13" s="75"/>
       <c r="I13" s="58" t="s">
         <v>26</v>
       </c>
@@ -5314,7 +5150,7 @@
     </row>
     <row r="14" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6"/>
-      <c r="B14" s="72"/>
+      <c r="B14" s="76"/>
       <c r="C14" s="59" t="s">
         <v>8</v>
       </c>
@@ -5325,7 +5161,7 @@
         <v>0.86114869475585598</v>
       </c>
       <c r="F14" s="25"/>
-      <c r="H14" s="72"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="59" t="s">
         <v>8</v>
       </c>
@@ -5342,7 +5178,7 @@
     </row>
     <row r="15" spans="1:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11"/>
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="74" t="s">
         <v>22</v>
       </c>
       <c r="C15" s="57" t="s">
@@ -5357,7 +5193,7 @@
       <c r="F15" s="17">
         <v>65.182065859908803</v>
       </c>
-      <c r="H15" s="70" t="s">
+      <c r="H15" s="74" t="s">
         <v>22</v>
       </c>
       <c r="I15" s="57" t="s">
@@ -5382,7 +5218,7 @@
     </row>
     <row r="16" spans="1:16" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="11"/>
-      <c r="B16" s="71"/>
+      <c r="B16" s="75"/>
       <c r="C16" s="58" t="s">
         <v>26</v>
       </c>
@@ -5395,7 +5231,7 @@
       <c r="F16" s="23">
         <v>0.99999999999998301</v>
       </c>
-      <c r="H16" s="71"/>
+      <c r="H16" s="75"/>
       <c r="I16" s="58" t="s">
         <v>26</v>
       </c>
@@ -5417,7 +5253,7 @@
       <c r="O16" s="39"/>
     </row>
     <row r="17" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="72"/>
+      <c r="B17" s="76"/>
       <c r="C17" s="59" t="s">
         <v>8</v>
       </c>
@@ -5428,7 +5264,7 @@
         <v>0.999998682044413</v>
       </c>
       <c r="F17" s="25"/>
-      <c r="H17" s="72"/>
+      <c r="H17" s="76"/>
       <c r="I17" s="59" t="s">
         <v>8</v>
       </c>
@@ -5445,7 +5281,7 @@
     </row>
     <row r="18" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="70" t="s">
+      <c r="B18" s="74" t="s">
         <v>25</v>
       </c>
       <c r="C18" s="57" t="s">
@@ -5460,7 +5296,7 @@
       <c r="F18" s="17">
         <v>402.71211179796398</v>
       </c>
-      <c r="H18" s="70" t="s">
+      <c r="H18" s="74" t="s">
         <v>25</v>
       </c>
       <c r="I18" s="57" t="s">
@@ -5484,7 +5320,7 @@
       <c r="O18" s="39"/>
     </row>
     <row r="19" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B19" s="71"/>
+      <c r="B19" s="75"/>
       <c r="C19" s="58" t="s">
         <v>26</v>
       </c>
@@ -5497,7 +5333,7 @@
       <c r="F19" s="23">
         <v>1</v>
       </c>
-      <c r="H19" s="71"/>
+      <c r="H19" s="75"/>
       <c r="I19" s="58" t="s">
         <v>26</v>
       </c>
@@ -5519,7 +5355,7 @@
       <c r="O19" s="39"/>
     </row>
     <row r="20" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="72"/>
+      <c r="B20" s="76"/>
       <c r="C20" s="59" t="s">
         <v>8</v>
       </c>
@@ -5530,7 +5366,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="25"/>
-      <c r="H20" s="72"/>
+      <c r="H20" s="76"/>
       <c r="I20" s="59" t="s">
         <v>8</v>
       </c>
@@ -5547,7 +5383,7 @@
     </row>
     <row r="21" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="74" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="57" t="s">
@@ -5562,7 +5398,7 @@
       <c r="F21" s="26">
         <v>1.6023121272854099E-4</v>
       </c>
-      <c r="H21" s="70" t="s">
+      <c r="H21" s="74" t="s">
         <v>27</v>
       </c>
       <c r="I21" s="57" t="s">
@@ -5587,7 +5423,7 @@
     </row>
     <row r="22" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="11"/>
-      <c r="B22" s="71"/>
+      <c r="B22" s="75"/>
       <c r="C22" s="58" t="s">
         <v>26</v>
       </c>
@@ -5600,7 +5436,7 @@
       <c r="F22" s="23">
         <v>1</v>
       </c>
-      <c r="H22" s="71"/>
+      <c r="H22" s="75"/>
       <c r="I22" s="58" t="s">
         <v>26</v>
       </c>
@@ -5622,7 +5458,7 @@
       <c r="O22" s="39"/>
     </row>
     <row r="23" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="72"/>
+      <c r="B23" s="76"/>
       <c r="C23" s="59" t="s">
         <v>8</v>
       </c>
@@ -5633,7 +5469,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="25"/>
-      <c r="H23" s="72"/>
+      <c r="H23" s="76"/>
       <c r="I23" s="59" t="s">
         <v>8</v>
       </c>
@@ -5650,7 +5486,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="74" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="57" t="s">
@@ -5665,7 +5501,7 @@
       <c r="F24" s="17">
         <v>3.2932556854758501</v>
       </c>
-      <c r="H24" s="70" t="s">
+      <c r="H24" s="74" t="s">
         <v>29</v>
       </c>
       <c r="I24" s="57" t="s">
@@ -5690,7 +5526,7 @@
     </row>
     <row r="25" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="11"/>
-      <c r="B25" s="71"/>
+      <c r="B25" s="75"/>
       <c r="C25" s="58" t="s">
         <v>26</v>
       </c>
@@ -5703,7 +5539,7 @@
       <c r="F25" s="23">
         <v>0.94671514952184899</v>
       </c>
-      <c r="H25" s="71"/>
+      <c r="H25" s="75"/>
       <c r="I25" s="58" t="s">
         <v>26</v>
       </c>
@@ -5725,7 +5561,7 @@
       <c r="O25" s="39"/>
     </row>
     <row r="26" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="72"/>
+      <c r="B26" s="76"/>
       <c r="C26" s="59" t="s">
         <v>8</v>
       </c>
@@ -5736,7 +5572,7 @@
         <v>0.681479053631181</v>
       </c>
       <c r="F26" s="25"/>
-      <c r="H26" s="72"/>
+      <c r="H26" s="76"/>
       <c r="I26" s="59" t="s">
         <v>8</v>
       </c>
@@ -5752,7 +5588,7 @@
       <c r="O26" s="39"/>
     </row>
     <row r="27" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="70" t="s">
+      <c r="B27" s="74" t="s">
         <v>32</v>
       </c>
       <c r="C27" s="57" t="s">
@@ -5767,7 +5603,7 @@
       <c r="F27" s="17">
         <v>2.0350314610621099</v>
       </c>
-      <c r="H27" s="70" t="s">
+      <c r="H27" s="74" t="s">
         <v>32</v>
       </c>
       <c r="I27" s="57" t="s">
@@ -5790,7 +5626,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="71"/>
+      <c r="B28" s="75"/>
       <c r="C28" s="58" t="s">
         <v>26</v>
       </c>
@@ -5803,7 +5639,7 @@
       <c r="F28" s="23">
         <v>0.99840659133647602</v>
       </c>
-      <c r="H28" s="71"/>
+      <c r="H28" s="75"/>
       <c r="I28" s="58" t="s">
         <v>26</v>
       </c>
@@ -5824,7 +5660,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="72"/>
+      <c r="B29" s="76"/>
       <c r="C29" s="59" t="s">
         <v>8</v>
       </c>
@@ -5835,7 +5671,7 @@
         <v>0.887186941951009</v>
       </c>
       <c r="F29" s="25"/>
-      <c r="H29" s="72"/>
+      <c r="H29" s="76"/>
       <c r="I29" s="59" t="s">
         <v>8</v>
       </c>
@@ -5892,29 +5728,19 @@
       <c r="C39" s="1"/>
     </row>
     <row r="70" spans="17:18" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q70" s="66" t="s">
+      <c r="Q70" s="70" t="s">
         <v>35</v>
       </c>
-      <c r="R70" s="67"/>
+      <c r="R70" s="71"/>
     </row>
     <row r="71" spans="17:18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q71" s="68" t="s">
+      <c r="Q71" s="72" t="s">
         <v>36</v>
       </c>
-      <c r="R71" s="69"/>
+      <c r="R71" s="73"/>
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="H12:H14"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="H3:H5"/>
-    <mergeCell ref="H6:H8"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="H9:H11"/>
     <mergeCell ref="Q70:R70"/>
     <mergeCell ref="Q71:R71"/>
     <mergeCell ref="B27:B29"/>
@@ -5931,6 +5757,16 @@
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="B21:B23"/>
     <mergeCell ref="H21:H23"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="H12:H14"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="H3:H5"/>
+    <mergeCell ref="H6:H8"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="H9:H11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>